<commit_message>
Actualizaciones generales: scripts de teams, templates y archivos de excel
</commit_message>
<xml_diff>
--- a/archivos/EstudiantesNuevosIA.xlsx
+++ b/archivos/EstudiantesNuevosIA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\aprovisionamientoEstudiantes\archivos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\App_Aprovicionamiento_M365\archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0DE8199C-BB25-4DCB-B8BF-50E12C09B53D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFCE79C4-7237-433E-8F64-62833EE94145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{1909EA82-7CFD-4791-9F6C-C4381A27CC70}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1909EA82-7CFD-4791-9F6C-C4381A27CC70}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -630,12 +630,12 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.77734375" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -673,14 +673,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="str">
-        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
-        <v>Estudiante - Transicion: Rozo Pineda Daniel Santiago</v>
-      </c>
-      <c r="B2" s="2" t="str">
-        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
-        <v>40302011@calasanzsuba.edu.co</v>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="e">
+        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B2" s="2" t="e">
+        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
+        <v>#REF!</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>12</v>
@@ -713,14 +713,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" t="str">
-        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
-        <v>Estudiante - Primero: Sanchez Mosquera Paula Alejandra</v>
-      </c>
-      <c r="B3" t="str">
-        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
-        <v>40302012@calasanzsuba.edu.co</v>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="e">
+        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B3" t="e">
+        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
+        <v>#REF!</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
@@ -753,14 +753,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="str">
-        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
-        <v>Estudiante - Segundo: Sarmiento Cantor Miguel Santiago</v>
-      </c>
-      <c r="B4" s="2" t="str">
-        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
-        <v>40302013@calasanzsuba.edu.co</v>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="e">
+        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B4" s="2" t="e">
+        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
+        <v>#REF!</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>24</v>
@@ -793,14 +793,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" t="str">
-        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
-        <v xml:space="preserve">Estudiante - Tercero: Serna Ballesteros Alejandra </v>
-      </c>
-      <c r="B5" t="str">
-        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
-        <v>40302014@calasanzsuba.edu.co</v>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="e">
+        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B5" t="e">
+        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
+        <v>#REF!</v>
       </c>
       <c r="C5" t="s">
         <v>27</v>
@@ -833,14 +833,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="str">
-        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
-        <v xml:space="preserve">Estudiante - Cuarto: Tellez Pedraza Valentina </v>
-      </c>
-      <c r="B6" s="2" t="str">
-        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
-        <v>40302015@calasanzsuba.edu.co</v>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="e">
+        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B6" s="2" t="e">
+        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
+        <v>#REF!</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>31</v>
@@ -873,14 +873,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" t="str">
-        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
-        <v>Estudiante - Quinto: Usma Niño Maria Paula</v>
-      </c>
-      <c r="B7" t="str">
-        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
-        <v>40302016@calasanzsuba.edu.co</v>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="e">
+        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B7" t="e">
+        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
+        <v>#REF!</v>
       </c>
       <c r="C7" t="s">
         <v>34</v>
@@ -913,14 +913,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="str">
-        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
-        <v>Estudiante - Sexto: Valbuena Gamboa Erick Santiago</v>
-      </c>
-      <c r="B8" s="2" t="str">
-        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
-        <v>40302017@calasanzsuba.edu.co</v>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="e">
+        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B8" s="2" t="e">
+        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
+        <v>#REF!</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>37</v>
@@ -953,14 +953,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" t="str">
-        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
-        <v>Estudiante - Septimo: Velasquez Ortiz Cristian David</v>
-      </c>
-      <c r="B9" t="str">
-        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
-        <v>40302018@calasanzsuba.edu.co</v>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="e">
+        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B9" t="e">
+        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
+        <v>#REF!</v>
       </c>
       <c r="C9" t="s">
         <v>41</v>
@@ -993,14 +993,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="str">
-        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
-        <v xml:space="preserve">Estudiante - Octavo: Vera Molano Nicolas </v>
-      </c>
-      <c r="B10" s="2" t="str">
-        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
-        <v>40302019@calasanzsuba.edu.co</v>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="e">
+        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B10" s="2" t="e">
+        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
+        <v>#REF!</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>44</v>
@@ -1033,14 +1033,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" t="str">
-        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
-        <v>Estudiante - Undécimo: Villamil Molina German Alfonso</v>
-      </c>
-      <c r="B11" t="str">
-        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
-        <v>40302020@calasanzsuba.edu.co</v>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="e">
+        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B11" t="e">
+        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
+        <v>#REF!</v>
       </c>
       <c r="C11" t="s">
         <v>47</v>
@@ -1070,14 +1070,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="str">
-        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
-        <v>Estudiante - Transicion: Sarmiento Cantor Maria Paula</v>
-      </c>
-      <c r="B12" s="2" t="str">
-        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
-        <v>40302021@calasanzsuba.edu.co</v>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="e">
+        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B12" s="2" t="e">
+        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
+        <v>#REF!</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>34</v>
@@ -1110,14 +1110,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" t="str">
-        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
-        <v>Estudiante - Primero: Serna Ballesteros Erick Santiago</v>
-      </c>
-      <c r="B13" t="str">
-        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
-        <v>40302022@calasanzsuba.edu.co</v>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="e">
+        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B13" t="e">
+        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
+        <v>#REF!</v>
       </c>
       <c r="C13" t="s">
         <v>37</v>
@@ -1150,14 +1150,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="str">
-        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
-        <v>Estudiante - Segundo: Tellez Pedraza Cristian David</v>
-      </c>
-      <c r="B14" s="2" t="str">
-        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
-        <v>40302023@calasanzsuba.edu.co</v>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="e">
+        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B14" s="2" t="e">
+        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
+        <v>#REF!</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>41</v>
@@ -1190,14 +1190,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" t="str">
-        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
-        <v xml:space="preserve">Estudiante - Tercero: Usma Niño Nicolas </v>
-      </c>
-      <c r="B15" t="str">
-        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
-        <v>40302024@calasanzsuba.edu.co</v>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="e">
+        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B15" t="e">
+        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
+        <v>#REF!</v>
       </c>
       <c r="C15" t="s">
         <v>44</v>
@@ -1230,14 +1230,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="str">
-        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
-        <v>Estudiante - Cuarto: Villamil Molina Dany Ernesto</v>
-      </c>
-      <c r="B16" s="2" t="str">
-        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
-        <v>40302025@calasanzsuba.edu.co</v>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="e">
+        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B16" s="2" t="e">
+        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
+        <v>#REF!</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>50</v>
@@ -1270,14 +1270,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" t="str">
-        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
-        <v>Estudiante - Quinto: Sarmiento Cantor German Alfonso</v>
-      </c>
-      <c r="B17" t="str">
-        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
-        <v>40302026@calasanzsuba.edu.co</v>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="e">
+        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B17" t="e">
+        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
+        <v>#REF!</v>
       </c>
       <c r="C17" t="s">
         <v>47</v>
@@ -1310,14 +1310,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="str">
-        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
-        <v>Estudiante - Sexto: Serna Ballesteros Maria Paula</v>
-      </c>
-      <c r="B18" s="2" t="str">
-        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
-        <v>40302027@calasanzsuba.edu.co</v>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="e">
+        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B18" s="2" t="e">
+        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
+        <v>#REF!</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>34</v>
@@ -1350,14 +1350,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" t="str">
-        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
-        <v>Estudiante - Septimo: Tellez Pedraza Erick Santiago</v>
-      </c>
-      <c r="B19" t="str">
-        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
-        <v>40302028@calasanzsuba.edu.co</v>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="e">
+        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B19" t="e">
+        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
+        <v>#REF!</v>
       </c>
       <c r="C19" t="s">
         <v>37</v>
@@ -1390,14 +1390,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="str">
-        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
-        <v>Estudiante - Octavo: Usma Niño Cristian David</v>
-      </c>
-      <c r="B20" s="2" t="str">
-        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
-        <v>40302029@calasanzsuba.edu.co</v>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="e">
+        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B20" s="2" t="e">
+        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
+        <v>#REF!</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>41</v>
@@ -1430,14 +1430,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" t="str">
-        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
-        <v xml:space="preserve">Estudiante - Undécimo: Sarmiento Cantor Nicolas </v>
-      </c>
-      <c r="B21" t="str">
-        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
-        <v>40302030@calasanzsuba.edu.co</v>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="e">
+        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B21" t="e">
+        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
+        <v>#REF!</v>
       </c>
       <c r="C21" t="s">
         <v>44</v>
@@ -1467,14 +1467,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="str">
-        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
-        <v>Estudiante - Transicion: Serna Ballesteros German Alfonso</v>
-      </c>
-      <c r="B22" s="2" t="str">
-        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
-        <v>40302031@calasanzsuba.edu.co</v>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="e">
+        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B22" s="2" t="e">
+        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
+        <v>#REF!</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>47</v>
@@ -1507,14 +1507,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" t="str">
-        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
-        <v>Estudiante - Primero: Rozo Pineda Cristian David</v>
-      </c>
-      <c r="B23" t="str">
-        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
-        <v>40302032@calasanzsuba.edu.co</v>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="e">
+        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B23" t="e">
+        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
+        <v>#REF!</v>
       </c>
       <c r="C23" t="s">
         <v>41</v>
@@ -1547,14 +1547,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="str">
-        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
-        <v xml:space="preserve">Estudiante - Segundo: Sanchez Mosquera Nicolas </v>
-      </c>
-      <c r="B24" s="2" t="str">
-        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
-        <v>40302033@calasanzsuba.edu.co</v>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="e">
+        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B24" s="2" t="e">
+        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
+        <v>#REF!</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>44</v>
@@ -1587,14 +1587,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A25" t="str">
-        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
-        <v>Estudiante - Tercero: Sarmiento Cantor German Alfonso</v>
-      </c>
-      <c r="B25" t="str">
-        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
-        <v>40302034@calasanzsuba.edu.co</v>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" t="e">
+        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B25" t="e">
+        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
+        <v>#REF!</v>
       </c>
       <c r="C25" t="s">
         <v>47</v>
@@ -1627,14 +1627,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="str">
-        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
-        <v>Estudiante - Cuarto: Serna Ballesteros Maria Andrea</v>
-      </c>
-      <c r="B26" s="2" t="str">
-        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
-        <v>40302035@calasanzsuba.edu.co</v>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="e">
+        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B26" s="2" t="e">
+        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
+        <v>#REF!</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>51</v>
@@ -1667,14 +1667,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A27" t="str">
-        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
-        <v>Estudiante - Quinto: Valbuena Gamboa Miguel Santiago</v>
-      </c>
-      <c r="B27" t="str">
-        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
-        <v>40302036@calasanzsuba.edu.co</v>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="e">
+        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B27" t="e">
+        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
+        <v>#REF!</v>
       </c>
       <c r="C27" t="s">
         <v>24</v>
@@ -1707,14 +1707,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="str">
-        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
-        <v xml:space="preserve">Estudiante - Sexto: Velasquez Ortiz Alejandra </v>
-      </c>
-      <c r="B28" s="2" t="str">
-        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
-        <v>40302037@calasanzsuba.edu.co</v>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="e">
+        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B28" s="2" t="e">
+        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
+        <v>#REF!</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>27</v>
@@ -1747,14 +1747,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" t="str">
-        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
-        <v>Estudiante - Septimo: Velasquez Ortiz Miguel Santiago</v>
-      </c>
-      <c r="B29" t="str">
-        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
-        <v>40302038@calasanzsuba.edu.co</v>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" t="e">
+        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B29" t="e">
+        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
+        <v>#REF!</v>
       </c>
       <c r="C29" t="s">
         <v>24</v>
@@ -1787,14 +1787,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A30" s="8" t="str">
-        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
-        <v xml:space="preserve">Estudiante - Octavo: Vera Molano Alejandra </v>
-      </c>
-      <c r="B30" s="8" t="str">
-        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
-        <v>40302039@calasanzsuba.edu.co</v>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="e">
+        <f>_xlfn.CONCAT("Estudiante - ",[1]!estudiantes[[#This Row],[GRADO]],": ",[1]!estudiantes[[#This Row],[APELLIDOS]]," ",[1]!estudiantes[[#This Row],[NOMBRES]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B30" s="8" t="e">
+        <f>_xlfn.CONCAT([1]!estudiantes[[#This Row],[CODIGO]],"@calasanzsuba.edu.co")</f>
+        <v>#REF!</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>27</v>

</xml_diff>